<commit_message>
Tawarruq --App Data entry - Application details, Customer Details & DocumentDetails testcase updated
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_Tawruqq/TestData/TawruqqTestData.xlsx
+++ b/AzentioAutomationFramework_Tawruqq/TestData/TawruqqTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="23256" windowHeight="12600" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="ijara_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="560">
   <si>
     <t>UserName</t>
   </si>
@@ -1200,9 +1200,6 @@
     <t>DS_AT_TW_AD_06</t>
   </si>
   <si>
-    <t>Chennai</t>
-  </si>
-  <si>
     <t>Pondi</t>
   </si>
   <si>
@@ -1714,6 +1711,9 @@
   </si>
   <si>
     <t>4224</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
   </si>
 </sst>
 </file>
@@ -2538,15 +2538,15 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" width="19.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2671,16 +2671,16 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.44140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="24" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2794,16 +2794,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="30" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="35" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2886,41 +2886,41 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.6640625" style="3" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24" style="3" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="47.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="47.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.88671875" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.88671875" style="3" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="24" style="3" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="31.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="31.28515625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="31.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="31.33203125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.6640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="24" style="3" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="29" max="29" width="31.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.6640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.44140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -3365,20 +3365,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3470,11 +3470,11 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3510,21 +3510,21 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3639,18 +3639,18 @@
       <c r="G5" s="47"/>
       <c r="H5" s="46"/>
       <c r="I5" s="46" t="s">
+        <v>559</v>
+      </c>
+      <c r="J5" s="46" t="s">
         <v>388</v>
-      </c>
-      <c r="J5" s="46" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>390</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>391</v>
       </c>
       <c r="C6" s="46" t="s">
         <v>367</v>
@@ -3673,22 +3673,22 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4180,33 +4180,33 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>352</v>
+      <c r="A44" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>354</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="B45" s="42" t="s">
-        <v>354</v>
+      <c r="A45" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>356</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>356</v>
+      <c r="A46" s="45" t="s">
+        <v>377</v>
+      </c>
+      <c r="B46" s="45" t="s">
+        <v>378</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>60</v>
@@ -4214,10 +4214,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="45" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B47" s="45" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>60</v>
@@ -4225,10 +4225,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="45" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B48" s="45" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>60</v>
@@ -4236,40 +4236,29 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="45" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="45" t="s">
-        <v>351</v>
-      </c>
-      <c r="B50" s="45" t="s">
-        <v>387</v>
+      <c r="A50" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="B50" s="48" t="s">
+        <v>390</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="48" t="s">
-        <v>390</v>
-      </c>
-      <c r="B51" s="48" t="s">
-        <v>391</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4284,27 +4273,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4318,60 +4307,60 @@
         <v>369</v>
       </c>
       <c r="D1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" t="s">
         <v>392</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>393</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>394</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>395</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>396</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>397</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>398</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>399</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>400</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>401</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>402</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>403</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>404</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>405</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>406</v>
-      </c>
-      <c r="S1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="49" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>408</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>409</v>
       </c>
       <c r="C2">
         <v>3393</v>
@@ -4382,10 +4371,10 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="49" t="s">
+        <v>409</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>410</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>411</v>
       </c>
       <c r="C3">
         <v>3393</v>
@@ -4397,10 +4386,10 @@
         <v>13000</v>
       </c>
       <c r="F3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G3" t="s">
         <v>412</v>
-      </c>
-      <c r="G3" t="s">
-        <v>413</v>
       </c>
       <c r="H3">
         <v>85000</v>
@@ -4412,16 +4401,16 @@
         <v>164</v>
       </c>
       <c r="L3" t="s">
+        <v>413</v>
+      </c>
+      <c r="M3" t="s">
         <v>414</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>415</v>
       </c>
-      <c r="N3" t="s">
-        <v>416</v>
-      </c>
       <c r="O3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P3">
         <v>1500</v>
@@ -4430,24 +4419,24 @@
         <v>100</v>
       </c>
       <c r="R3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="49" t="s">
+        <v>417</v>
+      </c>
+      <c r="B4" s="50" t="s">
         <v>418</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>419</v>
       </c>
       <c r="C4">
         <v>3393</v>
       </c>
       <c r="F4" t="s">
+        <v>419</v>
+      </c>
+      <c r="G4" t="s">
         <v>420</v>
-      </c>
-      <c r="G4" t="s">
-        <v>421</v>
       </c>
       <c r="H4">
         <v>58000</v>
@@ -4456,16 +4445,16 @@
         <v>100</v>
       </c>
       <c r="L4" t="s">
+        <v>421</v>
+      </c>
+      <c r="M4" t="s">
         <v>422</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>423</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>424</v>
-      </c>
-      <c r="O4" t="s">
-        <v>425</v>
       </c>
       <c r="P4">
         <v>750</v>
@@ -4476,10 +4465,10 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="49" t="s">
+        <v>425</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>426</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>427</v>
       </c>
       <c r="C5">
         <v>3393</v>
@@ -4491,18 +4480,18 @@
         <v>18500</v>
       </c>
       <c r="F5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="49" t="s">
+        <v>428</v>
+      </c>
+      <c r="B6" s="50" t="s">
         <v>429</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>430</v>
       </c>
       <c r="C6">
         <v>3393</v>
@@ -4514,24 +4503,24 @@
         <v>8950</v>
       </c>
       <c r="F6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H6">
         <v>22000</v>
       </c>
       <c r="I6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="49" t="s">
+        <v>431</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>432</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>433</v>
       </c>
       <c r="C7">
         <v>3393</v>
@@ -4539,27 +4528,27 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="49" t="s">
+        <v>433</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>434</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>435</v>
       </c>
       <c r="C8">
         <v>3393</v>
       </c>
       <c r="R8" t="s">
+        <v>435</v>
+      </c>
+      <c r="S8" t="s">
         <v>436</v>
-      </c>
-      <c r="S8" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>438</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>439</v>
       </c>
       <c r="C9">
         <v>3393</v>
@@ -4578,23 +4567,23 @@
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4608,60 +4597,60 @@
         <v>369</v>
       </c>
       <c r="D1" t="s">
+        <v>439</v>
+      </c>
+      <c r="E1" t="s">
         <v>440</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>441</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>442</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>443</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>444</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>445</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>446</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>447</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>448</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>405</v>
+      </c>
+      <c r="O1" t="s">
         <v>449</v>
       </c>
-      <c r="N1" t="s">
-        <v>406</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>450</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>451</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>452</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>453</v>
-      </c>
-      <c r="S1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B2" t="s">
         <v>455</v>
-      </c>
-      <c r="B2" t="s">
-        <v>456</v>
       </c>
       <c r="C2">
         <v>3016</v>
@@ -4669,34 +4658,34 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" t="s">
         <v>457</v>
-      </c>
-      <c r="B3" t="s">
-        <v>458</v>
       </c>
       <c r="C3">
         <v>3016</v>
       </c>
       <c r="D3" t="s">
+        <v>458</v>
+      </c>
+      <c r="E3" t="s">
         <v>459</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>460</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>461</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>462</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>463</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>464</v>
-      </c>
-      <c r="J3" t="s">
-        <v>465</v>
       </c>
       <c r="K3">
         <v>1000000</v>
@@ -4708,47 +4697,47 @@
         <v>60000</v>
       </c>
       <c r="N3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B4" t="s">
         <v>467</v>
-      </c>
-      <c r="B4" t="s">
-        <v>468</v>
       </c>
       <c r="C4">
         <v>3016</v>
       </c>
       <c r="E4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Q4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B5" t="s">
         <v>469</v>
-      </c>
-      <c r="B5" t="s">
-        <v>470</v>
       </c>
       <c r="C5">
         <v>3016</v>
       </c>
       <c r="R5" t="s">
+        <v>452</v>
+      </c>
+      <c r="S5" t="s">
         <v>453</v>
-      </c>
-      <c r="S5" t="s">
-        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4764,11 +4753,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4779,15 +4768,15 @@
         <v>196</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="50" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>472</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>473</v>
       </c>
       <c r="C2" s="1">
         <v>3620</v>
@@ -4795,10 +4784,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="50" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>474</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>475</v>
       </c>
       <c r="C3" s="1">
         <v>3620</v>
@@ -4806,10 +4795,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="50" t="s">
+        <v>475</v>
+      </c>
+      <c r="B4" s="50" t="s">
         <v>476</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>477</v>
       </c>
       <c r="C4" s="1">
         <v>3620</v>
@@ -4817,10 +4806,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="50" t="s">
+        <v>477</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>478</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>479</v>
       </c>
       <c r="C5" s="1">
         <v>3620</v>
@@ -4840,23 +4829,23 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="18" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="38" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
@@ -5072,23 +5061,23 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="28.8">
       <c r="A1" s="51" t="s">
         <v>195</v>
       </c>
@@ -5096,7 +5085,7 @@
         <v>196</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D1" s="51" t="s">
         <v>357</v>
@@ -5128,13 +5117,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="50" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>481</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="C2" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="D2" s="50">
         <v>450</v>
@@ -5174,32 +5163,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -5207,7 +5196,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C1" s="55" t="s">
         <v>369</v>
@@ -5219,63 +5208,63 @@
         <v>149</v>
       </c>
       <c r="F1" s="55" t="s">
+        <v>496</v>
+      </c>
+      <c r="G1" s="55" t="s">
         <v>497</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="H1" s="55" t="s">
         <v>498</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="I1" s="55" t="s">
         <v>499</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="J1" s="55" t="s">
         <v>500</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="K1" s="55" t="s">
         <v>501</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="L1" s="55" t="s">
         <v>502</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="M1" s="55" t="s">
         <v>503</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="N1" s="55" t="s">
         <v>504</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="O1" s="55" t="s">
         <v>505</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="P1" s="55" t="s">
         <v>506</v>
       </c>
-      <c r="P1" s="55" t="s">
+      <c r="Q1" s="55" t="s">
         <v>507</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="R1" s="55" t="s">
         <v>508</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="S1" s="55" t="s">
         <v>509</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="T1" s="55" t="s">
         <v>510</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="U1" s="55" t="s">
         <v>511</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="V1" s="55" t="s">
         <v>512</v>
-      </c>
-      <c r="V1" s="55" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>514</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>515</v>
       </c>
       <c r="C2" s="7">
         <v>2971</v>
@@ -5302,17 +5291,17 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>516</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>517</v>
       </c>
       <c r="C3" s="7">
         <v>2971</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -5334,19 +5323,19 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -5368,39 +5357,39 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>523</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>120</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>527</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>528</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>226</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N5" s="7">
         <v>123</v>
@@ -5409,19 +5398,19 @@
         <v>123</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>533</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>534</v>
       </c>
       <c r="U5" s="7">
         <v>5</v>
@@ -5432,20 +5421,20 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>536</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -5464,39 +5453,39 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>539</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>544</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>545</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>226</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N7" s="7">
         <v>456</v>
@@ -5505,19 +5494,19 @@
         <v>456</v>
       </c>
       <c r="P7" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q7" s="7" t="s">
         <v>547</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="S7" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>550</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>551</v>
       </c>
       <c r="U7" s="7">
         <v>7</v>
@@ -5528,20 +5517,20 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>553</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -5560,13 +5549,13 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>556</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
@@ -5590,19 +5579,19 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>559</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -5640,15 +5629,15 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5772,44 +5761,44 @@
       <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="62.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="62.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="31.33203125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="35.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="30.44140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.88671875" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="23" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="20.44140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="17.5546875" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="17" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.44140625" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="22.33203125" customWidth="1" collapsed="1"/>
     <col min="34" max="34" width="18" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -6472,36 +6461,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="20" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="18" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.6640625" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="21" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="33.5546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="23.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -6932,17 +6921,17 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="53" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="53" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="53" customWidth="1"/>
     <col min="4" max="5" width="27" style="53" customWidth="1"/>
     <col min="6" max="1024" width="11" style="53" customWidth="1"/>
-    <col min="1025" max="16384" width="10.28515625" style="53"/>
+    <col min="1025" max="16384" width="10.33203125" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75">
+    <row r="1" spans="1:14" ht="15.6">
       <c r="A1" s="52" t="s">
         <v>7</v>
       </c>
@@ -6953,25 +6942,25 @@
         <v>369</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>370</v>
       </c>
       <c r="F1" s="53" t="s">
+        <v>484</v>
+      </c>
+      <c r="G1" s="53" t="s">
         <v>485</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="H1" s="53" t="s">
         <v>486</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>487</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>130</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K1" s="53" t="s">
         <v>133</v>
@@ -6980,13 +6969,13 @@
         <v>137</v>
       </c>
       <c r="M1" s="53" t="s">
+        <v>488</v>
+      </c>
+      <c r="N1" s="53" t="s">
         <v>489</v>
       </c>
-      <c r="N1" s="53" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75">
+    </row>
+    <row r="2" spans="1:14" ht="15.6">
       <c r="A2" s="52" t="s">
         <v>233</v>
       </c>
@@ -6997,19 +6986,19 @@
         <v>3877</v>
       </c>
       <c r="D2" s="53" t="s">
+        <v>490</v>
+      </c>
+      <c r="E2" s="54" t="s">
         <v>491</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="F2" s="54" t="s">
         <v>492</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>493</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>125</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I2" s="54" t="s">
         <v>129</v>
@@ -7021,10 +7010,10 @@
         <v>134</v>
       </c>
       <c r="L2" s="54" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.6">
       <c r="A3" s="52" t="s">
         <v>238</v>
       </c>
@@ -7035,16 +7024,16 @@
         <v>3877</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M3" s="54" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N3" s="53" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.6">
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
     </row>
@@ -7066,37 +7055,37 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="21" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.88671875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.44140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.6640625" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="19" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.44140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="20.5546875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="21.109375" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="23" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="18.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -7531,24 +7520,24 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.5546875" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="23" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -7833,19 +7822,19 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>